<commit_message>
Correção ortográfica nos gráficos
Correção ortográfica nos gráficos de consultas
</commit_message>
<xml_diff>
--- a/Dados/Graficos Consulta/consultas filtrado.xlsx
+++ b/Dados/Graficos Consulta/consultas filtrado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Área de Trabalho\fatec\API\Dados\Graficos Consulta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fatec\Desktop\API\Dados\Graficos Consulta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD73CC61-B972-43AE-8C40-EDD3E9032EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B006C0D9-B170-4B79-9273-67B4226494A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aparecida" sheetId="1" r:id="rId1"/>
@@ -81,11 +81,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -145,7 +145,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR"/>
-              <a:t>consultas específicas  em Aparecida</a:t>
+              <a:t>Consultas específicas  em Aparecida</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -702,7 +702,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>tota de consultas  em </a:t>
+              <a:t>Total de consultas  em </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="pt-BR"/>
@@ -1584,7 +1584,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>aparecida!$C$2</c15:sqref>
@@ -1611,7 +1611,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>aparecida!$A$3:$A$6</c15:sqref>
@@ -1638,7 +1638,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>aparecida!$C$3:$C$6</c15:sqref>
@@ -1660,7 +1660,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-93EC-4C40-BD70-A6A9F45084EB}"/>
                   </c:ext>
@@ -1981,7 +1981,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>consultas específicas  em Taubaté</a:t>
+              <a:t>Consultas específicas  em Taubaté</a:t>
             </a:r>
             <a:endParaRPr lang="pt-BR" sz="1400"/>
           </a:p>
@@ -2545,7 +2545,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>tota de consultas em Taubaté</a:t>
+              <a:t>Total de consultas em Taubaté</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2824,7 +2824,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Taubaté!$C$2</c15:sqref>
@@ -2851,7 +2851,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Taubaté!$A$3:$A$6</c15:sqref>
@@ -2878,7 +2878,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Taubaté!$C$3:$C$6</c15:sqref>
@@ -2900,7 +2900,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-8B25-44A5-AA07-0F03B5866AD6}"/>
                   </c:ext>
@@ -3235,7 +3235,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>consultas específicas  em Caçapava</a:t>
+              <a:t>Consultas específicas  em Caçapava</a:t>
             </a:r>
             <a:endParaRPr lang="pt-BR" sz="1800"/>
           </a:p>
@@ -3806,7 +3806,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>total de consultas  em Caçapava</a:t>
+              <a:t>Total de consultas  em Caçapava</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1400"/>
           </a:p>
@@ -4086,7 +4086,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>caçapava!$C$2</c15:sqref>
@@ -4113,7 +4113,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>caçapava!$A$3:$A$6</c15:sqref>
@@ -4140,7 +4140,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>caçapava!$C$3:$C$6</c15:sqref>
@@ -4162,7 +4162,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-BC2D-4AAD-A648-9B36A9B11434}"/>
                   </c:ext>
@@ -4499,7 +4499,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>consultas específicas  em </a:t>
+              <a:t>Consultas específicas  em </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="pt-BR" baseline="0"/>
@@ -5074,7 +5074,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>tota de consultas  em </a:t>
+              <a:t>Total de consultas  em </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="pt-BR" baseline="0"/>
@@ -5677,7 +5677,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>consultas específicas  em </a:t>
+              <a:t>Consultas específicas  em </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="pt-BR"/>
@@ -11911,15 +11911,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:colOff>495300</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12293,27 +12293,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -12324,7 +12324,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -12332,7 +12332,7 @@
         <v>16494</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -12346,7 +12346,7 @@
         <v>36313</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -12360,7 +12360,7 @@
         <v>56243</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -12391,23 +12391,23 @@
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -12418,15 +12418,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>228437</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -12436,11 +12436,11 @@
       <c r="C4">
         <v>264</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>272837</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -12450,11 +12450,11 @@
       <c r="C5">
         <v>296</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>181974</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -12464,7 +12464,7 @@
       <c r="C6">
         <v>1032</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>241334</v>
       </c>
     </row>
@@ -12485,23 +12485,23 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -12511,11 +12511,11 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -12523,7 +12523,7 @@
         <v>55622</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -12537,7 +12537,7 @@
         <v>76831</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -12551,7 +12551,7 @@
         <v>104642</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -12583,23 +12583,23 @@
       <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -12610,7 +12610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -12618,7 +12618,7 @@
         <v>392281</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -12632,7 +12632,7 @@
         <v>398007</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -12646,7 +12646,7 @@
         <v>309336</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -12673,27 +12673,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADEC6CFC-9D4E-4F65-BD28-65808C56B3D2}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -12704,15 +12704,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>1148261</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -12722,11 +12722,11 @@
       <c r="C4">
         <v>1963</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>587322</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -12736,11 +12736,11 @@
       <c r="C5">
         <v>652</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>850975</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -12750,12 +12750,12 @@
       <c r="C6">
         <v>968</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>741974</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E12" s="3"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>